<commit_message>
work on establishing pfm pyomo model
</commit_message>
<xml_diff>
--- a/input files/hpp_layout.xlsx
+++ b/input files/hpp_layout.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s203679_dtu_dk/Documents/Dokumenter/DTU (studies)/speciale/Speciale/input files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bluepp-my.sharepoint.com/personal/xfsf_bpp-projects_com/Documents/Documents/GitHub/Speciale/input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{3A720C2A-8BB2-46CC-9A31-194013BDD676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC822D62-1222-4D30-A09F-D716DCF0E133}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{3A720C2A-8BB2-46CC-9A31-194013BDD676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B674D15-1E61-449C-868C-1791E5818BA2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7643C590-AB87-4ECC-9949-F1DE609BD7D2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{7643C590-AB87-4ECC-9949-F1DE609BD7D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Carriers" sheetId="3" r:id="rId1"/>
-    <sheet name="Buses" sheetId="4" r:id="rId2"/>
-    <sheet name="Components" sheetId="1" r:id="rId3"/>
-    <sheet name="Contracts" sheetId="2" r:id="rId4"/>
+    <sheet name="Components" sheetId="1" r:id="rId2"/>
+    <sheet name="Contracts" sheetId="2" r:id="rId3"/>
+    <sheet name="PPAs" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
     <author>Frederik Skou Fertin</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D8A9701D-5B57-471A-8F0C-1C9A2CC863BC}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{D8A9701D-5B57-471A-8F0C-1C9A2CC863BC}">
       <text>
         <r>
           <rPr>
@@ -72,8 +72,76 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Frederik Skou Fertin</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{80B8BD84-C120-4CF8-9CBF-A99A73B6A1C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Frederik Skou Fertin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+€/t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Frederik Skou Fertin</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{81CBFBB2-BCE5-440F-9F42-480A77FB4E74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Frederik Skou Fertin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+€/MWh</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>Electrolyzer</t>
   </si>
@@ -183,36 +251,18 @@
     <t>volume</t>
   </si>
   <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>penalty</t>
-  </si>
-  <si>
-    <t>Hydrogen Offtake Agreement</t>
-  </si>
-  <si>
     <t>hourly</t>
   </si>
   <si>
     <t>Contract for selling H₂...</t>
   </si>
   <si>
-    <t>Ammonia Offtake Agreement</t>
-  </si>
-  <si>
     <t>yearly</t>
   </si>
   <si>
     <t>Contract for selling NH₃...</t>
   </si>
   <si>
-    <t>info</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
     <t>hydrogen_offtake</t>
   </si>
   <si>
@@ -231,9 +281,6 @@
     <t>nuclear</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>supplier</t>
   </si>
   <si>
@@ -247,15 +294,54 @@
   </si>
   <si>
     <t>default_unit</t>
+  </si>
+  <si>
+    <t>annual_cf</t>
+  </si>
+  <si>
+    <t>baseload ppa</t>
+  </si>
+  <si>
+    <t>Hydrogen1</t>
+  </si>
+  <si>
+    <t>Ammonia1</t>
+  </si>
+  <si>
+    <t>target_frequency</t>
+  </si>
+  <si>
+    <t>shipment_frequency</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>capacity_unit</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>kt H2</t>
+  </si>
+  <si>
+    <t>kt H2/h</t>
+  </si>
+  <si>
+    <t>kt NH3</t>
+  </si>
+  <si>
+    <t>kt NH3/h</t>
+  </si>
+  <si>
+    <t>grid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,7 +372,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +391,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -333,12 +431,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,80 +778,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94580FE-4FAA-4EB4-9011-2CE5D705C8AE}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.6328125" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="5" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -754,345 +837,439 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AE35B6-9C04-42B1-9A0C-9F8A3C1F5D9B}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4227C92-656E-4719-8EA9-FD34C0DD0C21}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="10" width="15.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2">
+        <v>400</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2">
+        <v>200</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
+        <f>480*G6</f>
+        <v>8.9887640449438209</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="G6" s="6">
+        <f>1/53.4</f>
+        <v>1.8726591760299626E-2</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <f>1200/24</f>
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>45</v>
+      <c r="G9" s="6">
+        <f>5.29</f>
+        <v>5.29</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <f>1200*50</f>
+        <v>60000</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2">
+        <v>60000</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:F11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4227C92-656E-4719-8EA9-FD34C0DD0C21}">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D653FE9-ECBC-4C18-ACB0-A1757BCB2761}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="15.6328125" customWidth="1"/>
+    <col min="1" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="C1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>10</v>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
-        <v>400</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>4000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>7.5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2">
-        <v>200</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>900</v>
+      </c>
+      <c r="D3" s="2">
+        <v>87600</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2">
-        <v>50</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="7">
-        <f>480*F6</f>
-        <v>8.9887640449438209</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="6">
-        <f>1/53.4</f>
-        <v>1.8726591760299626E-2</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2">
-        <f>1200/24</f>
-        <v>50</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="2">
-        <f>1/5.29</f>
-        <v>0.1890359168241966</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2">
-        <f>1200*50</f>
-        <v>60000</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1102,88 +1279,123 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D653FE9-ECBC-4C18-ACB0-A1757BCB2761}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2159F0F7-3B2A-4D06-AB40-89B8755A542A}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="15.6328125" customWidth="1"/>
+    <col min="1" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2000</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>200</v>
+      </c>
+      <c r="E2" s="2">
+        <v>40</v>
       </c>
       <c r="F2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2">
-        <v>300</v>
+        <v>0.4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="2">
-        <v>87600</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>400</v>
+      </c>
+      <c r="E3" s="2">
+        <v>25</v>
       </c>
       <c r="F3" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2">
+        <v>80</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactoring and simulation tool development
</commit_message>
<xml_diff>
--- a/input files/hpp_layout.xlsx
+++ b/input files/hpp_layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bluepp-my.sharepoint.com/personal/xfsf_bpp-projects_com/Documents/Documents/GitHub/Speciale/input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{3A720C2A-8BB2-46CC-9A31-194013BDD676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B674D15-1E61-449C-868C-1791E5818BA2}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="8_{3A720C2A-8BB2-46CC-9A31-194013BDD676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB28E63E-AB98-4B8F-A7BF-225727873BFF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{7643C590-AB87-4ECC-9949-F1DE609BD7D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7643C590-AB87-4ECC-9949-F1DE609BD7D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Carriers" sheetId="3" r:id="rId1"/>
@@ -64,7 +64,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-MWh/product</t>
+MWh/input</t>
         </r>
       </text>
     </comment>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>Electrolyzer</t>
   </si>
@@ -323,19 +323,22 @@
     <t>MW</t>
   </si>
   <si>
-    <t>kt H2</t>
-  </si>
-  <si>
-    <t>kt H2/h</t>
-  </si>
-  <si>
-    <t>kt NH3</t>
-  </si>
-  <si>
-    <t>kt NH3/h</t>
-  </si>
-  <si>
     <t>grid</t>
+  </si>
+  <si>
+    <t>AmmoniaSpot</t>
+  </si>
+  <si>
+    <t>t H2/h</t>
+  </si>
+  <si>
+    <t>t H2</t>
+  </si>
+  <si>
+    <t>t NH3/h</t>
+  </si>
+  <si>
+    <t>t NH3</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -440,10 +443,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,6 +458,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4227C92-656E-4719-8EA9-FD34C0DD0C21}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -970,7 +973,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2">
         <v>1000</v>
@@ -1007,7 +1010,7 @@
         <v>8.9887640449438209</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -1036,7 +1039,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
@@ -1064,7 +1067,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>20</v>
@@ -1095,7 +1098,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>20</v>
@@ -1104,12 +1107,12 @@
         <v>28</v>
       </c>
       <c r="G9" s="6">
-        <f>5.29</f>
-        <v>5.29</v>
+        <v>5.5</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
-        <v>0.3</v>
+        <f>0.3*G9</f>
+        <v>1.65</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>29</v>
@@ -1123,11 +1126,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="2">
-        <f>1200*50</f>
-        <v>60000</v>
+        <v>25000</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>28</v>
@@ -1139,7 +1141,9 @@
         <v>1</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2">
+        <v>1E-4</v>
+      </c>
       <c r="J10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1152,10 +1156,10 @@
         <v>47</v>
       </c>
       <c r="C11" s="2">
-        <v>60000</v>
+        <v>25000</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>28</v>
@@ -1192,23 +1196,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D653FE9-ECBC-4C18-ACB0-A1757BCB2761}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>34</v>
@@ -1222,22 +1231,20 @@
       <c r="F1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2">
         <v>4000</v>
       </c>
       <c r="D2" s="2">
-        <v>7.5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>36</v>
@@ -1254,7 +1261,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2">
         <v>900</v>
@@ -1271,6 +1278,28 @@
       <c r="G3" s="2" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2">
+        <v>500</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1280,9 +1309,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2159F0F7-3B2A-4D06-AB40-89B8755A542A}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1321,7 +1350,7 @@
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1345,7 +1374,7 @@
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1369,7 +1398,7 @@
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1390,9 +1419,6 @@
       <c r="H4" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>